<commit_message>
Refs 2:  - Compare data to detect changed row  - Process data to convert to json.txt  - Merge data to replace or add book in exist file
</commit_message>
<xml_diff>
--- a/data/compare/changes_report.xlsx
+++ b/data/compare/changes_report.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Changed Books" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Added Books" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Changed Books" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,6 +426,297 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price (vnd)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Discount (%)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Sold</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Rating</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Publisher</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Authors</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Other_sellers</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Bản Đồ (New Edition)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://tiki.vn/product-p50685547.html?spid=50685549</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>224250</v>
+      </c>
+      <c r="D2" t="n">
+        <v>35</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5935</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>['Nhã Nam']</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['Nhà Xuất Bản Lao Động']</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>['Aleksandra Mizielińska', 'Daniel Mizieliński']</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[{'name': 'nha sach nguyet linh', 'price': 325000, 'link': 'https://tiki.vn/cua-hang/nha-sach-nguyet-linh'}, {'name': 'AHABOOKS', 'price': 310500, 'link': 'https://tiki.vn/cua-hang/ahabooks'}, {'name': 'Nhà Sách Trẻ Online', 'price': 344310, 'link': 'https://tiki.vn/cua-hang/nha-sach-tre-online'}, {'name': 'Phương Đông Books', 'price': 299500, 'link': 'https://tiki.vn/cua-hang/phuong-dong-books'}, {'name': 'HaAnBooks', 'price': 345000, 'link': 'https://tiki.vn/cua-hang/haanbooks'}, {'name': 'Nhà Sách Vĩnh Thụy', 'price': 311000, 'link': 'https://tiki.vn/cua-hang/nha-sach-vinh-thuy'}, {'name': 'Alpha Books Official', 'price': 276000, 'link': 'https://tiki.vn/cua-hang/alphabooks-official'}, {'name': 'SÁCH ĐẠI NAM', 'price': 340000, 'link': 'https://tiki.vn/cua-hang/sach-dai-nam'}, {'name': 'Sống Official', 'price': 276000, 'link': 'https://tiki.vn/cua-hang/abcbooks'}, {'name': 'Việt Thư Books', 'price': 327750, 'link': 'https://tiki.vn/cua-hang/viet-thu-books'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Thiên Tài Bên Trái, Kẻ Điên Bên Phải (Tái Bản) (New Edition)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://tiki.vn/product-p109017985.html?spid=109017987</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>110980</v>
+      </c>
+      <c r="D3" t="n">
+        <v>38</v>
+      </c>
+      <c r="E3" t="n">
+        <v>25756</v>
+      </c>
+      <c r="F3" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>['Vibooks']</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['Nhà Xuất Bản Thế Giới']</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>['Cao Minh']</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[{'name': 'Skybooks Official Store', 'price': 161100, 'link': 'https://tiki.vn/cua-hang/skybooks-official-store'}, {'name': 'Tazano Official Store', 'price': 143000, 'link': 'https://tiki.vn/cua-hang/sachbanchay'}, {'name': 'AHABOOKS', 'price': 166351, 'link': 'https://tiki.vn/cua-hang/ahabooks'}, {'name': 'VBooks', 'price': 179000, 'link': 'https://tiki.vn/cua-hang/vbooks'}, {'name': 'Minhhabooks', 'price': 126000, 'link': 'https://tiki.vn/cua-hang/minhhabooks'}, {'name': 'Bamboo Books', 'price': 161100, 'link': 'https://tiki.vn/cua-hang/bamboo-books'}, {'name': 'Omega Plus Books', 'price': 143000, 'link': 'https://tiki.vn/cua-hang/omega-plus-books'}, {'name': 'Times Books', 'price': 151850, 'link': 'https://tiki.vn/cua-hang/times-books'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Yêu Những Ngày Nắng Chẳng Ghét Những Ngày Mưa (New Edition)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://tiki.vn/product-p190861557.html?spid=190861559</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>80520</v>
+      </c>
+      <c r="D4" t="n">
+        <v>39</v>
+      </c>
+      <c r="E4" t="n">
+        <v>5318</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['Skybooks']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['Nhà Xuất Bản Phụ Nữ']</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>['Kulzsc']</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>[{'name': 'AHABOOKS', 'price': 117500, 'link': 'https://tiki.vn/cua-hang/ahabooks'}, {'name': 'Nhà Sách Vĩnh Thụy', 'price': 132000, 'link': 'https://tiki.vn/cua-hang/nha-sach-vinh-thuy'}, {'name': 'Skybooks Official Store', 'price': 118800, 'link': 'https://tiki.vn/cua-hang/skybooks-official-store'}, {'name': 'Times Books', 'price': 111900, 'link': 'https://tiki.vn/cua-hang/times-books'}, {'name': 'SÁCH ĐẠI NAM', 'price': 132000, 'link': 'https://tiki.vn/cua-hang/sach-dai-nam'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Càng Kỷ Luật, Càng Tự Do (New Edition)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://tiki.vn/product-p68585576.html?spid=68585577</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>65400</v>
+      </c>
+      <c r="D5" t="n">
+        <v>40</v>
+      </c>
+      <c r="E5" t="n">
+        <v>21225</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['Bloom Books']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['Nhà Xuất Bản Thế Giới']</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>['Ca Tây']</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>[{'name': 'Nhà sách Fahasa', 'price': 96000, 'link': 'https://tiki.vn/cua-hang/nha-sach-fahasa'}, {'name': 'Skybooks Official Store', 'price': 98100, 'link': 'https://tiki.vn/cua-hang/skybooks-official-store'}, {'name': 'Nhà Sách Trẻ Online', 'price': 92050, 'link': 'https://tiki.vn/cua-hang/nha-sach-tre-online'}, {'name': 'Phương Đông Books', 'price': 99500, 'link': 'https://tiki.vn/cua-hang/phuong-dong-books'}, {'name': 'Times Books', 'price': 92350, 'link': 'https://tiki.vn/cua-hang/times-books'}, {'name': 'Omega Plus Books', 'price': 87000, 'link': 'https://tiki.vn/cua-hang/omega-plus-books'}, {'name': 'Nhà Sách Vĩnh Thụy', 'price': 98000, 'link': 'https://tiki.vn/cua-hang/nha-sach-vinh-thuy'}, {'name': 'Alpha Books Official', 'price': 87000, 'link': 'https://tiki.vn/cua-hang/alphabooks-official'}, {'name': 'VBooks', 'price': 109000, 'link': 'https://tiki.vn/cua-hang/vbooks'}, {'name': 'NHBook', 'price': 93000, 'link': 'https://tiki.vn/cua-hang/nhbook'}, {'name': 'Việt Thư Books', 'price': 103550, 'link': 'https://tiki.vn/cua-hang/viet-thu-books'}, {'name': 'info book', 'price': 98000, 'link': 'https://tiki.vn/cua-hang/info-book'}]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Dear, Darling (New Edition)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://tiki.vn/product-p174444163.html?spid=174444165</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>58960</v>
+      </c>
+      <c r="D6" t="n">
+        <v>33</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6084</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['Skybooks']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['Nhà Xuất Bản Phụ Nữ Việt Nam']</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>['Hiên']</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>[{'name': 'Skybooks Official Store', 'price': 79200, 'link': 'https://tiki.vn/cua-hang/skybooks-official-store'}, {'name': 'NewShop Official', 'price': 70400, 'link': 'https://tiki.vn/cua-hang/newshopvn'}, {'name': 'Tazano Official Store', 'price': 68000, 'link': 'https://tiki.vn/cua-hang/sachbanchay'}, {'name': 'Phương Đông Books', 'price': 88000, 'link': 'https://tiki.vn/cua-hang/phuong-dong-books'}, {'name': 'AHABOOKS', 'price': 88000, 'link': 'https://tiki.vn/cua-hang/ahabooks'}, {'name': 'Nhà Sách Vĩnh Thụy', 'price': 88000, 'link': 'https://tiki.vn/cua-hang/nha-sach-vinh-thuy'}, {'name': 'info book', 'price': 88000, 'link': 'https://tiki.vn/cua-hang/info-book'}, {'name': 'ETS Books', 'price': 66000, 'link': 'https://tiki.vn/cua-hang/ets-books'}, {'name': 'Nhà Sách Trẻ Online', 'price': 74200, 'link': 'https://tiki.vn/cua-hang/nha-sach-tre-online'}, {'name': 'Times Books', 'price': 74500, 'link': 'https://tiki.vn/cua-hang/times-books'}]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>